<commit_message>
table modified for envfit
</commit_message>
<xml_diff>
--- a/samples.xlsx
+++ b/samples.xlsx
@@ -15,12 +15,12 @@
     <sheet name="samples" sheetId="1" r:id="rId1"/>
     <sheet name="mensi" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="250">
   <si>
     <t>id</t>
   </si>
@@ -703,12 +703,6 @@
     <t>VOJ111</t>
   </si>
   <si>
-    <t>16177_2</t>
-  </si>
-  <si>
-    <t>VOJ112</t>
-  </si>
-  <si>
     <t>16122_1</t>
   </si>
   <si>
@@ -770,6 +764,12 @@
   </si>
   <si>
     <t>pH</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -1594,15 +1594,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1616,10 +1616,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1635,8 +1641,14 @@
       <c r="E2">
         <v>4.45</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>0.48</v>
+      </c>
+      <c r="G2">
+        <v>44.76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1652,8 +1664,14 @@
       <c r="E3">
         <v>4.95</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G3">
+        <v>47.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1669,8 +1687,14 @@
       <c r="E4">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G4">
+        <v>47.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1686,8 +1710,14 @@
       <c r="E5">
         <v>4.17</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>0.12</v>
+      </c>
+      <c r="G5">
+        <v>49.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1703,8 +1733,14 @@
       <c r="E6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G6">
+        <v>53.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1720,8 +1756,14 @@
       <c r="E7">
         <v>4.97</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>0.505</v>
+      </c>
+      <c r="G7">
+        <v>47.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1737,8 +1779,14 @@
       <c r="E8">
         <v>5.42</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>0.21</v>
+      </c>
+      <c r="G8">
+        <v>46.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1754,8 +1802,14 @@
       <c r="E9">
         <v>5.95</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G9">
+        <v>45.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1771,8 +1825,14 @@
       <c r="E10">
         <v>3.45</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>0.17</v>
+      </c>
+      <c r="G10">
+        <v>50.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1788,8 +1848,14 @@
       <c r="E11">
         <v>4.37</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="G11">
+        <v>50.57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1805,8 +1871,14 @@
       <c r="E12">
         <v>4.17</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G12">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1822,8 +1894,14 @@
       <c r="E13">
         <v>4.55</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="G13">
+        <v>43.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1839,8 +1917,14 @@
       <c r="E14">
         <v>4.29</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="G14">
+        <v>51.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1856,8 +1940,14 @@
       <c r="E15">
         <v>3.84</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="G15">
+        <v>53.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1873,8 +1963,14 @@
       <c r="E16">
         <v>3.63</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="G16">
+        <v>51.77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1890,8 +1986,14 @@
       <c r="E17">
         <v>3.49</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="G17">
+        <v>50.39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1907,8 +2009,14 @@
       <c r="E18">
         <v>3.86</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="G18">
+        <v>54.29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1924,8 +2032,14 @@
       <c r="E19">
         <v>4.0599999999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="G19">
+        <v>51.23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1941,8 +2055,14 @@
       <c r="E20">
         <v>3.54</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>0.43</v>
+      </c>
+      <c r="G20">
+        <v>53.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1958,8 +2078,14 @@
       <c r="E21">
         <v>4.88</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="G21">
+        <v>49.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1975,8 +2101,14 @@
       <c r="E22">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="G22">
+        <v>51.53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1992,8 +2124,14 @@
       <c r="E23">
         <v>4.09</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>0.111</v>
+      </c>
+      <c r="G23">
+        <v>51.65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2009,8 +2147,14 @@
       <c r="E24">
         <v>4.24</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G24">
+        <v>49.19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -2026,8 +2170,14 @@
       <c r="E25">
         <v>4.8899999999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G25">
+        <v>48.71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2043,8 +2193,14 @@
       <c r="E26">
         <v>3.62</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G26">
+        <v>51.35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2060,8 +2216,14 @@
       <c r="E27">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>0.153</v>
+      </c>
+      <c r="G27">
+        <v>47.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -2077,8 +2239,14 @@
       <c r="E28">
         <v>3.45</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="G28">
+        <v>46.19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2094,8 +2262,14 @@
       <c r="E29">
         <v>4.6900000000000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <v>1.389</v>
+      </c>
+      <c r="G29">
+        <v>44.94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -2111,8 +2285,14 @@
       <c r="E30">
         <v>4.62</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="G30">
+        <v>50.03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2128,8 +2308,14 @@
       <c r="E31">
         <v>4.04</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G31">
+        <v>48.71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -2145,8 +2331,14 @@
       <c r="E32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="G32">
+        <v>48.11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -2162,8 +2354,14 @@
       <c r="E33">
         <v>4.01</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <v>0.376</v>
+      </c>
+      <c r="G33">
+        <v>52.37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -2179,8 +2377,14 @@
       <c r="E34">
         <v>3.53</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="G34">
+        <v>50.93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -2196,8 +2400,14 @@
       <c r="E35">
         <v>3.46</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G35">
+        <v>55.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -2213,8 +2423,14 @@
       <c r="E36">
         <v>3.85</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G36">
+        <v>55.13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2230,8 +2446,14 @@
       <c r="E37">
         <v>3.73</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G37">
+        <v>53.99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -2247,8 +2469,14 @@
       <c r="E38">
         <v>3.72</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="G38">
+        <v>57.17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -2264,8 +2492,14 @@
       <c r="E39">
         <v>4.6500000000000004</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <v>0.39</v>
+      </c>
+      <c r="G39">
+        <v>52.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -2281,8 +2515,14 @@
       <c r="E40">
         <v>4.1500000000000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>0.91</v>
+      </c>
+      <c r="G40">
+        <v>48.65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2298,8 +2538,14 @@
       <c r="E41">
         <v>3.72</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <v>0.157</v>
+      </c>
+      <c r="G41">
+        <v>54.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2315,8 +2561,14 @@
       <c r="E42">
         <v>3.45</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <v>0.12</v>
+      </c>
+      <c r="G42">
+        <v>52.79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -2332,8 +2584,14 @@
       <c r="E43">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <v>0.19</v>
+      </c>
+      <c r="G43">
+        <v>53.51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2349,8 +2607,14 @@
       <c r="E44">
         <v>3.69</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="G44">
+        <v>50.03</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -2366,8 +2630,14 @@
       <c r="E45">
         <v>4.83</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G45">
+        <v>48.71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -2383,8 +2653,14 @@
       <c r="E46">
         <v>4.66</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <v>0.122</v>
+      </c>
+      <c r="G46">
+        <v>44.09</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>97</v>
       </c>
@@ -2400,8 +2676,14 @@
       <c r="E47">
         <v>4.58</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="G47">
+        <v>39.409999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -2417,8 +2699,14 @@
       <c r="E48">
         <v>5.37</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G48">
+        <v>40.01</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>101</v>
       </c>
@@ -2434,8 +2722,14 @@
       <c r="E49">
         <v>4.25</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <v>0.106</v>
+      </c>
+      <c r="G49">
+        <v>43.01</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -2451,8 +2745,14 @@
       <c r="E50">
         <v>5.43</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="G50">
+        <v>42.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -2468,8 +2768,14 @@
       <c r="E51">
         <v>3.36</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G51">
+        <v>42.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -2485,8 +2791,14 @@
       <c r="E52">
         <v>3.16</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G52">
+        <v>41.33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2502,8 +2814,14 @@
       <c r="E53">
         <v>4.7699999999999996</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="G53">
+        <v>43.13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -2519,8 +2837,14 @@
       <c r="E54">
         <v>3.46</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="G54">
+        <v>50.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -2536,8 +2860,14 @@
       <c r="E55">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <v>0.154</v>
+      </c>
+      <c r="G55">
+        <v>38.69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -2553,8 +2883,14 @@
       <c r="E56">
         <v>4.41</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="G56">
+        <v>44.99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -2570,8 +2906,14 @@
       <c r="E57">
         <v>4.38</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G57">
+        <v>44.21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>119</v>
       </c>
@@ -2587,8 +2929,14 @@
       <c r="E58">
         <v>4.12</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="G58">
+        <v>44.27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -2604,8 +2952,14 @@
       <c r="E59">
         <v>4.5599999999999996</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>1.1739999999999999</v>
+      </c>
+      <c r="G59">
+        <v>47.09</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -2621,8 +2975,14 @@
       <c r="E60">
         <v>4.38</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="G60">
+        <v>41.21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -2638,8 +2998,14 @@
       <c r="E61">
         <v>3.84</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="G61">
+        <v>44.33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>127</v>
       </c>
@@ -2655,8 +3021,14 @@
       <c r="E62">
         <v>4.54</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <v>0.108</v>
+      </c>
+      <c r="G62">
+        <v>40.25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>129</v>
       </c>
@@ -2672,8 +3044,14 @@
       <c r="E63">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G63">
+        <v>47.09</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>131</v>
       </c>
@@ -2689,8 +3067,14 @@
       <c r="E64">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="G64">
+        <v>45.11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>133</v>
       </c>
@@ -2706,8 +3090,14 @@
       <c r="E65">
         <v>3.73</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <v>0.161</v>
+      </c>
+      <c r="G65">
+        <v>45.35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -2723,8 +3113,14 @@
       <c r="E66">
         <v>4.05</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G66">
+        <v>42.65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>137</v>
       </c>
@@ -2740,8 +3136,14 @@
       <c r="E67">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G67">
+        <v>43.79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -2757,8 +3159,14 @@
       <c r="E68">
         <v>4.1100000000000003</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="G68">
+        <v>49.31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -2774,8 +3182,14 @@
       <c r="E69">
         <v>3.13</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G69">
+        <v>45.47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -2791,8 +3205,14 @@
       <c r="E70">
         <v>5.52</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G70">
+        <v>38.450000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -2808,8 +3228,14 @@
       <c r="E71">
         <v>4.66</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G71">
+        <v>42.77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -2825,8 +3251,14 @@
       <c r="E72">
         <v>4.33</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="G72">
+        <v>45.41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -2842,8 +3274,14 @@
       <c r="E73">
         <v>5.62</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <v>0.122</v>
+      </c>
+      <c r="G73">
+        <v>40.07</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>151</v>
       </c>
@@ -2859,8 +3297,14 @@
       <c r="E74">
         <v>4.74</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G74">
+        <v>40.07</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -2876,8 +3320,14 @@
       <c r="E75">
         <v>3.93</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>0.374</v>
+      </c>
+      <c r="G75">
+        <v>50.75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>155</v>
       </c>
@@ -2893,8 +3343,14 @@
       <c r="E76">
         <v>4.29</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G76">
+        <v>43.55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -2910,8 +3366,14 @@
       <c r="E77">
         <v>3.82</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <v>0.107</v>
+      </c>
+      <c r="G77">
+        <v>45.23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>159</v>
       </c>
@@ -2927,8 +3389,14 @@
       <c r="E78">
         <v>3.82</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="G78">
+        <v>47.57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -2944,8 +3412,14 @@
       <c r="E79">
         <v>3.44</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="G79">
+        <v>49.85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>163</v>
       </c>
@@ -2961,8 +3435,14 @@
       <c r="E80">
         <v>3.54</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="G80">
+        <v>43.97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>165</v>
       </c>
@@ -2978,8 +3458,14 @@
       <c r="E81">
         <v>3.88</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <v>0.152</v>
+      </c>
+      <c r="G81">
+        <v>49.07</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>167</v>
       </c>
@@ -2995,8 +3481,14 @@
       <c r="E82">
         <v>3.46</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <v>0.65</v>
+      </c>
+      <c r="G82">
+        <v>47.39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>169</v>
       </c>
@@ -3012,8 +3504,14 @@
       <c r="E83">
         <v>3.15</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <v>0.189</v>
+      </c>
+      <c r="G83">
+        <v>46.37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>171</v>
       </c>
@@ -3029,8 +3527,14 @@
       <c r="E84">
         <v>4.6100000000000003</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="G84">
+        <v>41.15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -3046,8 +3550,14 @@
       <c r="E85">
         <v>3.32</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85">
+        <v>0.152</v>
+      </c>
+      <c r="G85">
+        <v>44.99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -3063,8 +3573,14 @@
       <c r="E86">
         <v>3.99</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="G86">
+        <v>46.85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>177</v>
       </c>
@@ -3080,8 +3596,14 @@
       <c r="E87">
         <v>5.54</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87">
+        <v>0.187</v>
+      </c>
+      <c r="G87">
+        <v>39.17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>179</v>
       </c>
@@ -3097,8 +3619,14 @@
       <c r="E88">
         <v>4.66</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G88">
+        <v>40.549999999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>181</v>
       </c>
@@ -3114,8 +3642,14 @@
       <c r="E89">
         <v>4.49</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G89">
+        <v>45.77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>183</v>
       </c>
@@ -3131,8 +3665,14 @@
       <c r="E90">
         <v>3.47</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G90">
+        <v>43.19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>185</v>
       </c>
@@ -3148,8 +3688,14 @@
       <c r="E91">
         <v>3.64</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="G91">
+        <v>51.77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>187</v>
       </c>
@@ -3165,8 +3711,14 @@
       <c r="E92">
         <v>3.13</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G92">
+        <v>45.11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>189</v>
       </c>
@@ -3182,8 +3734,14 @@
       <c r="E93">
         <v>3.78</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93">
+        <v>0.315</v>
+      </c>
+      <c r="G93">
+        <v>49.19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>191</v>
       </c>
@@ -3199,8 +3757,14 @@
       <c r="E94">
         <v>3.61</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94">
+        <v>0.629</v>
+      </c>
+      <c r="G94">
+        <v>45.17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>193</v>
       </c>
@@ -3216,8 +3780,14 @@
       <c r="E95">
         <v>4.58</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="G95">
+        <v>43.19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>195</v>
       </c>
@@ -3233,8 +3803,14 @@
       <c r="E96">
         <v>5.46</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G96">
+        <v>42.95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>197</v>
       </c>
@@ -3250,8 +3826,14 @@
       <c r="E97">
         <v>4.6100000000000003</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97">
+        <v>0.31</v>
+      </c>
+      <c r="G97">
+        <v>41.75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>199</v>
       </c>
@@ -3267,8 +3849,14 @@
       <c r="E98">
         <v>3.57</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98">
+        <v>1.746</v>
+      </c>
+      <c r="G98">
+        <v>42.11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>201</v>
       </c>
@@ -3284,8 +3872,14 @@
       <c r="E99">
         <v>3.47</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="G99">
+        <v>47.69</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>203</v>
       </c>
@@ -3301,8 +3895,14 @@
       <c r="E100">
         <v>4.6399999999999997</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G100">
+        <v>45.35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>205</v>
       </c>
@@ -3318,8 +3918,14 @@
       <c r="E101">
         <v>3.99</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101">
+        <v>0.621</v>
+      </c>
+      <c r="G101">
+        <v>48.83</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>207</v>
       </c>
@@ -3335,8 +3941,14 @@
       <c r="E102">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="G102">
+        <v>45.36</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>209</v>
       </c>
@@ -3352,8 +3964,14 @@
       <c r="E103">
         <v>6.36</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103">
+        <v>0.124</v>
+      </c>
+      <c r="G103">
+        <v>40.65</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>211</v>
       </c>
@@ -3369,8 +3987,14 @@
       <c r="E104">
         <v>3.58</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F104">
+        <v>0.871</v>
+      </c>
+      <c r="G104">
+        <v>41.38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>213</v>
       </c>
@@ -3386,8 +4010,14 @@
       <c r="E105">
         <v>3.78</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F105">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G105">
+        <v>44.58</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>215</v>
       </c>
@@ -3403,8 +4033,14 @@
       <c r="E106">
         <v>4.5199999999999996</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F106">
+        <v>0.157</v>
+      </c>
+      <c r="G106">
+        <v>41.62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>217</v>
       </c>
@@ -3420,8 +4056,14 @@
       <c r="E107">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F107">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="G107">
+        <v>48.02</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>219</v>
       </c>
@@ -3437,8 +4079,14 @@
       <c r="E108">
         <v>4.03</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F108">
+        <v>0.63</v>
+      </c>
+      <c r="G108">
+        <v>39.74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>221</v>
       </c>
@@ -3454,8 +4102,14 @@
       <c r="E109">
         <v>5.74</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F109">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="G109">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>223</v>
       </c>
@@ -3471,8 +4125,14 @@
       <c r="E110">
         <v>5.31</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F110">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="G110">
+        <v>41.62</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>225</v>
       </c>
@@ -3488,8 +4148,14 @@
       <c r="E111">
         <v>4.9400000000000004</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F111">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="G111">
+        <v>41.31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>227</v>
       </c>
@@ -3497,7 +4163,7 @@
         <v>228</v>
       </c>
       <c r="C112" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D112">
         <v>1975</v>
@@ -3505,8 +4171,14 @@
       <c r="E112">
         <v>3.99</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F112">
+        <v>0.95</v>
+      </c>
+      <c r="G112">
+        <v>43.19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>229</v>
       </c>
@@ -3522,8 +4194,14 @@
       <c r="E113">
         <v>3.55</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F113">
+        <v>0.158</v>
+      </c>
+      <c r="G113">
+        <v>42.95</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>231</v>
       </c>
@@ -3539,8 +4217,14 @@
       <c r="E114">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F114">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="G114">
+        <v>39.74</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>233</v>
       </c>
@@ -3551,13 +4235,19 @@
         <v>9</v>
       </c>
       <c r="D115">
-        <v>1975</v>
+        <v>2013</v>
       </c>
       <c r="E115">
         <v>4.09</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G115">
+        <v>44.64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>235</v>
       </c>
@@ -3565,16 +4255,22 @@
         <v>236</v>
       </c>
       <c r="C116" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D116">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="E116">
         <v>4.08</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F116">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G116">
+        <v>44.27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>237</v>
       </c>
@@ -3582,16 +4278,22 @@
         <v>238</v>
       </c>
       <c r="C117" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D117">
-        <v>2008</v>
+        <v>1975</v>
       </c>
       <c r="E117">
         <v>3.88</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F117">
+        <v>0.222</v>
+      </c>
+      <c r="G117">
+        <v>43.55</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>239</v>
       </c>
@@ -3602,13 +4304,19 @@
         <v>6</v>
       </c>
       <c r="D118">
-        <v>1975</v>
+        <v>2013</v>
       </c>
       <c r="E118">
         <v>4.55</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118">
+        <v>0.44</v>
+      </c>
+      <c r="G118">
+        <v>47.42</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>241</v>
       </c>
@@ -3619,13 +4327,19 @@
         <v>6</v>
       </c>
       <c r="D119">
-        <v>2013</v>
+        <v>1997</v>
       </c>
       <c r="E119">
         <v>4.1500000000000004</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F119">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G119">
+        <v>46.81</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>243</v>
       </c>
@@ -3636,13 +4350,19 @@
         <v>6</v>
       </c>
       <c r="D120">
-        <v>1997</v>
+        <v>2008</v>
       </c>
       <c r="E120">
         <v>4.26</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F120">
+        <v>0.151</v>
+      </c>
+      <c r="G120">
+        <v>43.49</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>245</v>
       </c>
@@ -3653,24 +4373,16 @@
         <v>6</v>
       </c>
       <c r="D121">
-        <v>2008</v>
+        <v>1997</v>
       </c>
       <c r="E121">
         <v>3.78</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>247</v>
-      </c>
-      <c r="B122" t="s">
-        <v>248</v>
-      </c>
-      <c r="C122" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122">
-        <v>1997</v>
+      <c r="F121">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="G121">
+        <v>45.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>